<commit_message>
Finished looking at alternate solutions.
</commit_message>
<xml_diff>
--- a/Excel_Challenge_491 - Draw A Hollow Half Pyramid.xlsx
+++ b/Excel_Challenge_491 - Draw A Hollow Half Pyramid.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01D145C-7739-4B9B-BD58-360B7D15E014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4463E0B-F8B0-4AC1-BDDB-333F58F8BF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Original" sheetId="1" r:id="rId1"/>
-    <sheet name="Alt" sheetId="2" r:id="rId2"/>
-    <sheet name="Alt2" sheetId="3" r:id="rId3"/>
-    <sheet name="Alt3" sheetId="4" r:id="rId4"/>
+    <sheet name="Alt" sheetId="2" r:id="rId1"/>
+    <sheet name="Alt2" sheetId="3" r:id="rId2"/>
+    <sheet name="Alt3" sheetId="4" r:id="rId3"/>
+    <sheet name="Alt4" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -61,12 +61,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>https://www.linkedin.com/in/excelbi/recent-activity/all/</t>
   </si>
   <si>
     <t>This solution is not complete</t>
+  </si>
+  <si>
+    <t>This is not a full array.</t>
   </si>
 </sst>
 </file>
@@ -129,186 +132,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>542164</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="A person in a suit and red shirt&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAF66485-6210-3BF1-587F-85F6E2E2DB76}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4203700" y="0"/>
-          <a:ext cx="2764664" cy="10058400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Thought Bubble: Cloud 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1876D551-03C9-4A1C-C21A-19CF73C22FB1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3117850" y="2235200"/>
-          <a:ext cx="2355850" cy="1416050"/>
-        </a:xfrm>
-        <a:prstGeom prst="cloudCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 18790"/>
-            <a:gd name="adj2" fmla="val -170131"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-IN" sz="1200" b="1"/>
-            <a:t>Draw</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-IN" sz="1200" b="1" baseline="0"/>
-            <a:t> hollow half pyramids for numbers given in column A.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-IN" sz="1200" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>459740</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>29631</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="A close-up of several logos&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F50C1AC2-A19D-46BF-84D3-D3E89C373732}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5556250" y="2908300"/>
-          <a:ext cx="1005840" cy="620181"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -573,163 +396,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="4.109375" customWidth="1"/>
-    <col min="3" max="16" width="3.44140625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="W1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1">
-        <v>3</v>
-      </c>
-      <c r="F16" s="1">
-        <v>4</v>
-      </c>
-      <c r="G16" s="1">
-        <v>5</v>
-      </c>
-      <c r="H16" s="1">
-        <v>6</v>
-      </c>
-      <c r="I16" s="1">
-        <v>7</v>
-      </c>
-      <c r="J16" s="1">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9502BC63-8537-4C5D-BB1C-4F15BF6653CA}">
   <dimension ref="A1:X26"/>
   <sheetViews>
@@ -1172,11 +838,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2933C3-0C79-4CBB-97F3-C3F1C0F23209}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
@@ -1618,7 +1284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753D537D-AFDA-446F-83AB-4747B021769F}">
   <dimension ref="A1:X23"/>
   <sheetViews>
@@ -2055,4 +1721,535 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB12" sqref="AB12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="4.109375" customWidth="1"/>
+    <col min="3" max="16" width="3.44140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q9" cm="1">
+        <f t="array" aca="1" ref="Q9:U13" ca="1">_xlfn.MAP(A1:INDIRECT("R" &amp;A2&amp;"C"&amp;A2,FALSE),_xlfn.LAMBDA(_xlpm.x,IF(COLUMN(_xlpm.x)=1,1,IF(COLUMN(_xlpm.x)=ROW(_xlpm.x),ROW(_xlpm.x),""))))</f>
+        <v>1</v>
+      </c>
+      <c r="R9" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S9" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T9" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U9" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="S10" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T10" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U10" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q11">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S11">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="T11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U11" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q12">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R12" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S12" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T12">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="U12" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q13">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R13" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S13" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T13" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U13">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1">
+        <v>7</v>
+      </c>
+      <c r="J16" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="17:24" x14ac:dyDescent="0.3">
+      <c r="Q17" cm="1">
+        <f t="array" aca="1" ref="Q17:X24" ca="1">_xlfn.MAP(A1:INDIRECT("R" &amp;A9&amp;"C"&amp;A9,FALSE),_xlfn.LAMBDA(_xlpm.x,IF(COLUMN(_xlpm.x)=1,1,IF(COLUMN(_xlpm.x)=ROW(_xlpm.x),ROW(_xlpm.x),""))))</f>
+        <v>1</v>
+      </c>
+      <c r="R17" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S17" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T17" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U17" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="V17" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="W17" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="X17" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="17:24" x14ac:dyDescent="0.3">
+      <c r="Q18">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="S18" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T18" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U18" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="V18" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="W18" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="X18" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="17:24" x14ac:dyDescent="0.3">
+      <c r="Q19">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R19" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S19">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="T19" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U19" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="V19" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="W19" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="X19" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="17:24" x14ac:dyDescent="0.3">
+      <c r="Q20">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R20" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S20" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T20">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="U20" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="V20" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="W20" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="X20" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="17:24" x14ac:dyDescent="0.3">
+      <c r="Q21">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R21" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S21" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T21" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U21">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="V21" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="W21" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="X21" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="17:24" x14ac:dyDescent="0.3">
+      <c r="Q22">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R22" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S22" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T22" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U22" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="V22">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="W22" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="X22" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="17:24" x14ac:dyDescent="0.3">
+      <c r="Q23">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R23" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S23" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T23" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U23" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="V23" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="W23">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+      <c r="X23" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="17:24" x14ac:dyDescent="0.3">
+      <c r="Q24">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="R24" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="S24" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="T24" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="U24" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="V24" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="W24" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="X24">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added my own function
</commit_message>
<xml_diff>
--- a/Excel_Challenge_491 - Draw A Hollow Half Pyramid.xlsx
+++ b/Excel_Challenge_491 - Draw A Hollow Half Pyramid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4463E0B-F8B0-4AC1-BDDB-333F58F8BF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50771F6B-97BA-4842-A99D-F04B966A7E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>https://www.linkedin.com/in/excelbi/recent-activity/all/</t>
   </si>
@@ -71,18 +71,28 @@
   <si>
     <t>This is not a full array.</t>
   </si>
+  <si>
+    <t>My Function</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -99,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,18 +117,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1725,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1976,7 +1998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Q17" cm="1">
         <f t="array" aca="1" ref="Q17:X24" ca="1">_xlfn.MAP(A1:INDIRECT("R" &amp;A9&amp;"C"&amp;A9,FALSE),_xlfn.LAMBDA(_xlpm.x,IF(COLUMN(_xlpm.x)=1,1,IF(COLUMN(_xlpm.x)=ROW(_xlpm.x),ROW(_xlpm.x),""))))</f>
         <v>1</v>
@@ -2010,7 +2032,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Q18">
         <f ca="1"/>
         <v>1</v>
@@ -2044,7 +2066,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Q19">
         <f ca="1"/>
         <v>1</v>
@@ -2078,7 +2100,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Q20">
         <f ca="1"/>
         <v>1</v>
@@ -2112,7 +2134,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Q21">
         <f ca="1"/>
         <v>1</v>
@@ -2146,7 +2168,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Q22">
         <f ca="1"/>
         <v>1</v>
@@ -2180,7 +2202,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Q23">
         <f ca="1"/>
         <v>1</v>
@@ -2214,7 +2236,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="Q24">
         <f ca="1"/>
         <v>1</v>
@@ -2246,6 +2268,419 @@
       <c r="X24">
         <f ca="1"/>
         <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Q29" cm="1">
+        <f t="array" ref="Q29:X36">_xlfn.LAMBDA(_xlpm.n,
+_xlfn.LET(
+_xlpm.s, _xlfn.SEQUENCE(_xlpm.n),
+_xlpm.fx, _xlfn.LAMBDA(_xlpm.rz, _xlfn.MAKEARRAY(1,_xlpm.n,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,_xlfn.SWITCH(TRUE,_xlpm.c=1,1,_xlpm.rz=_xlpm.n,_xlpm.c,_xlpm.rz=_xlpm.c,_xlpm.c,"")))),
+_xlfn.DROP(_xlfn.REDUCE("",_xlpm.s, _xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlpm.fx(_xlpm.v)))),1)
+)
+)(8)</f>
+        <v>1</v>
+      </c>
+      <c r="R29" t="str">
+        <v/>
+      </c>
+      <c r="S29" t="str">
+        <v/>
+      </c>
+      <c r="T29" t="str">
+        <v/>
+      </c>
+      <c r="U29" t="str">
+        <v/>
+      </c>
+      <c r="V29" t="str">
+        <v/>
+      </c>
+      <c r="W29" t="str">
+        <v/>
+      </c>
+      <c r="X29" t="str">
+        <v/>
+      </c>
+      <c r="Z29" t="b" cm="1">
+        <f t="array" ref="Z29:AG36">_xlfn.ANCHORARRAY(Q29)=C9:J16</f>
+        <v>1</v>
+      </c>
+      <c r="AA29" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB29" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC29" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD29" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE29" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF29" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>2</v>
+      </c>
+      <c r="S30" t="str">
+        <v/>
+      </c>
+      <c r="T30" t="str">
+        <v/>
+      </c>
+      <c r="U30" t="str">
+        <v/>
+      </c>
+      <c r="V30" t="str">
+        <v/>
+      </c>
+      <c r="W30" t="str">
+        <v/>
+      </c>
+      <c r="X30" t="str">
+        <v/>
+      </c>
+      <c r="Z30" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA30" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB30" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC30" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD30" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE30" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF30" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31" t="str">
+        <v/>
+      </c>
+      <c r="S31">
+        <v>3</v>
+      </c>
+      <c r="T31" t="str">
+        <v/>
+      </c>
+      <c r="U31" t="str">
+        <v/>
+      </c>
+      <c r="V31" t="str">
+        <v/>
+      </c>
+      <c r="W31" t="str">
+        <v/>
+      </c>
+      <c r="X31" t="str">
+        <v/>
+      </c>
+      <c r="Z31" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA31" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB31" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC31" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD31" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE31" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF31" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="R32" t="str">
+        <v/>
+      </c>
+      <c r="S32" t="str">
+        <v/>
+      </c>
+      <c r="T32">
+        <v>4</v>
+      </c>
+      <c r="U32" t="str">
+        <v/>
+      </c>
+      <c r="V32" t="str">
+        <v/>
+      </c>
+      <c r="W32" t="str">
+        <v/>
+      </c>
+      <c r="X32" t="str">
+        <v/>
+      </c>
+      <c r="Z32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="17:33" x14ac:dyDescent="0.3">
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="R33" t="str">
+        <v/>
+      </c>
+      <c r="S33" t="str">
+        <v/>
+      </c>
+      <c r="T33" t="str">
+        <v/>
+      </c>
+      <c r="U33">
+        <v>5</v>
+      </c>
+      <c r="V33" t="str">
+        <v/>
+      </c>
+      <c r="W33" t="str">
+        <v/>
+      </c>
+      <c r="X33" t="str">
+        <v/>
+      </c>
+      <c r="Z33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="17:33" x14ac:dyDescent="0.3">
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="R34" t="str">
+        <v/>
+      </c>
+      <c r="S34" t="str">
+        <v/>
+      </c>
+      <c r="T34" t="str">
+        <v/>
+      </c>
+      <c r="U34" t="str">
+        <v/>
+      </c>
+      <c r="V34">
+        <v>6</v>
+      </c>
+      <c r="W34" t="str">
+        <v/>
+      </c>
+      <c r="X34" t="str">
+        <v/>
+      </c>
+      <c r="Z34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="17:33" x14ac:dyDescent="0.3">
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="R35" t="str">
+        <v/>
+      </c>
+      <c r="S35" t="str">
+        <v/>
+      </c>
+      <c r="T35" t="str">
+        <v/>
+      </c>
+      <c r="U35" t="str">
+        <v/>
+      </c>
+      <c r="V35" t="str">
+        <v/>
+      </c>
+      <c r="W35">
+        <v>7</v>
+      </c>
+      <c r="X35" t="str">
+        <v/>
+      </c>
+      <c r="Z35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="17:33" x14ac:dyDescent="0.3">
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36">
+        <v>2</v>
+      </c>
+      <c r="S36">
+        <v>3</v>
+      </c>
+      <c r="T36">
+        <v>4</v>
+      </c>
+      <c r="U36">
+        <v>5</v>
+      </c>
+      <c r="V36">
+        <v>6</v>
+      </c>
+      <c r="W36">
+        <v>7</v>
+      </c>
+      <c r="X36">
+        <v>8</v>
+      </c>
+      <c r="Z36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG36" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>